<commit_message>
Template updates and license page updates
</commit_message>
<xml_diff>
--- a/input/images/DAK_core data dictionary_template_v2.1.xlsx
+++ b/input/images/DAK_core data dictionary_template_v2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/InternalComputableGuidelinesWorkingGroup/Shared Documents/General/11. SOP/L2 SOP (work in progress)/L2 templates/GitHub templates (external)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3218" documentId="8_{B5D96A79-F5A3-4E3C-9DBE-AABCA645CDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C54CBE-0812-44CA-BD9E-37BCE63E1BDD}"/>
+  <xr:revisionPtr revIDLastSave="3221" documentId="8_{B5D96A79-F5A3-4E3C-9DBE-AABCA645CDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ECBB490-9EBC-4F90-BC9E-0DE5B1D4ECFA}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,30 +102,6 @@
           </rPr>
           <t xml:space="preserve">
 Please provide in this table the list of all the data dictionary tabs. Add/remove rows and update the text in red as needed. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{0C64B67B-23DC-4573-AEAC-F89EF57CD1A4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Note for the author:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Please edit in the row above the text highlighted in red.</t>
         </r>
       </text>
     </comment>
@@ -5730,9 +5706,6 @@
     <t>[Activity ID]</t>
   </si>
   <si>
-    <t>Template Release Date: April 07, 2025</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -5804,14 +5777,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Organization] [year]</t>
+      <t>© World Health Organization 2025</t>
     </r>
     <r>
       <rPr>
@@ -5852,6 +5818,9 @@
 All reasonable precautions have been taken by WHO to verify the information contained in this publication. However, the published material is being distributed without warranty of any kind, either expressed or implied. The responsibility for the interpretation and use of the material lies with the reader. In no event shall WHO be liable for damages arising from its use.
 Any dispute arising from or relating to this license, including its validity, interpretation, or application, shall, unless amicably settled, be subject to conciliation. In the event the dispute is not resolved by conciliation within thirty (30) days, the dispute shall be settled by arbitration. The arbitration shall be conducted in accordance with the modalities to be agreed upon by the parties or, in the absence of agreement within thirty (30) days of written communication of the intent to commence arbitration, with the UNCITRAL Arbitration Rules. The parties shall accept the arbitral award as final.</t>
     </r>
+  </si>
+  <si>
+    <t>Template Release Date: April 14, 2025</t>
   </si>
 </sst>
 </file>
@@ -16444,7 +16413,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:J12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="13"/>
@@ -16478,7 +16447,7 @@
     </row>
     <row r="2" spans="1:10" s="21" customFormat="1" ht="54" customHeight="1">
       <c r="B2" s="225" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C2" s="225"/>
       <c r="D2" s="225"/>
@@ -16598,7 +16567,7 @@
     <row r="11" spans="1:10" ht="13.5" thickTop="1"/>
     <row r="12" spans="1:10" ht="232.5" customHeight="1">
       <c r="B12" s="216" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C12" s="217"/>
       <c r="D12" s="217"/>
@@ -16622,7 +16591,7 @@
     </row>
     <row r="14" spans="1:10" ht="14.5">
       <c r="B14" s="46" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -16635,7 +16604,7 @@
     </row>
     <row r="15" spans="1:10" ht="14.5">
       <c r="B15" s="46" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -16744,7 +16713,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="215" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1">
@@ -20832,7 +20801,7 @@
   <customSheetViews>
     <customSheetView guid="{F40DE62F-0414-4AAF-8AC2-945CC453F02F}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:AF263" xr:uid="{FB3125BB-CB44-4A4C-A1C1-09986448BDCF}"/>
+      <autoFilter ref="A1:AF263" xr:uid="{83F76FF3-6CA7-47F4-A9C0-97188A9888A3}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="423">
@@ -20856,6 +20825,10 @@
     <mergeCell ref="L69:L70"/>
     <mergeCell ref="M69:M70"/>
     <mergeCell ref="N69:N70"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="R1:AV1"/>
     <mergeCell ref="A59:Q59"/>
@@ -20932,10 +20905,10 @@
     <mergeCell ref="AT46:AT47"/>
     <mergeCell ref="AU46:AU47"/>
     <mergeCell ref="AV46:AV47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="AO46:AO47"/>
+    <mergeCell ref="AP46:AP47"/>
+    <mergeCell ref="AQ46:AQ47"/>
+    <mergeCell ref="AR46:AR47"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:H49"/>
     <mergeCell ref="I48:I49"/>
@@ -20945,10 +20918,6 @@
     <mergeCell ref="M48:M49"/>
     <mergeCell ref="N48:N49"/>
     <mergeCell ref="AN46:AN47"/>
-    <mergeCell ref="AO46:AO47"/>
-    <mergeCell ref="AP46:AP47"/>
-    <mergeCell ref="AQ46:AQ47"/>
-    <mergeCell ref="AR46:AR47"/>
     <mergeCell ref="AI46:AI47"/>
     <mergeCell ref="AJ46:AJ47"/>
     <mergeCell ref="AK46:AK47"/>
@@ -21197,6 +21166,16 @@
     <mergeCell ref="AA66:AA67"/>
     <mergeCell ref="AB66:AB67"/>
     <mergeCell ref="AC66:AC67"/>
+    <mergeCell ref="Y69:Y70"/>
+    <mergeCell ref="Z69:Z70"/>
+    <mergeCell ref="AA69:AA70"/>
+    <mergeCell ref="AB69:AB70"/>
+    <mergeCell ref="AC69:AC70"/>
+    <mergeCell ref="T69:T70"/>
+    <mergeCell ref="U69:U70"/>
+    <mergeCell ref="V69:V70"/>
+    <mergeCell ref="W69:W70"/>
+    <mergeCell ref="X69:X70"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D69:D70"/>
     <mergeCell ref="E69:E70"/>
@@ -21230,16 +21209,6 @@
     <mergeCell ref="AJ66:AJ67"/>
     <mergeCell ref="AK66:AK67"/>
     <mergeCell ref="AL66:AL67"/>
-    <mergeCell ref="Y69:Y70"/>
-    <mergeCell ref="Z69:Z70"/>
-    <mergeCell ref="AA69:AA70"/>
-    <mergeCell ref="AB69:AB70"/>
-    <mergeCell ref="AC69:AC70"/>
-    <mergeCell ref="T69:T70"/>
-    <mergeCell ref="U69:U70"/>
-    <mergeCell ref="V69:V70"/>
-    <mergeCell ref="W69:W70"/>
-    <mergeCell ref="X69:X70"/>
     <mergeCell ref="AI69:AI70"/>
     <mergeCell ref="AJ69:AJ70"/>
     <mergeCell ref="AK69:AK70"/>
@@ -27912,6 +27881,78 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="db15119c-9bb3-4b2d-aba7-a20f2bdcd107">
+      <UserInfo>
+        <DisplayName>BORG, Sarah Ann</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>DUVALL, Susan</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>RATANAPRAYUL, Natschja</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TITI-OFEI, Regina</DisplayName>
+        <AccountId>62</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>COSMAS, Leonard</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GAFFIELD, Mary Eluned</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>gndirangu</DisplayName>
+        <AccountId>103</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce1eb032-f7c0-42b6-914e-65a5c98ce8c4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="db15119c-9bb3-4b2d-aba7-a20f2bdcd107" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006553529D1FC6824CBA83EEDA5E51662C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd9d8df0be95803e7319e4e8fd6e517">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ce1eb032-f7c0-42b6-914e-65a5c98ce8c4" xmlns:ns3="db15119c-9bb3-4b2d-aba7-a20f2bdcd107" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e496dec2d1664ef4f95c2258d1ac145" ns2:_="" ns3:_="">
     <xsd:import namespace="ce1eb032-f7c0-42b6-914e-65a5c98ce8c4"/>
@@ -28166,79 +28207,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="db15119c-9bb3-4b2d-aba7-a20f2bdcd107">
-      <UserInfo>
-        <DisplayName>BORG, Sarah Ann</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>DUVALL, Susan</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>RATANAPRAYUL, Natschja</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TITI-OFEI, Regina</DisplayName>
-        <AccountId>62</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>COSMAS, Leonard</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GAFFIELD, Mary Eluned</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>gndirangu</DisplayName>
-        <AccountId>103</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce1eb032-f7c0-42b6-914e-65a5c98ce8c4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="db15119c-9bb3-4b2d-aba7-a20f2bdcd107" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{117D62C5-B693-4014-B24B-9D6D08B6151A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+    <ds:schemaRef ds:uri="db15119c-9bb3-4b2d-aba7-a20f2bdcd107"/>
+    <ds:schemaRef ds:uri="ce1eb032-f7c0-42b6-914e-65a5c98ce8c4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B327EE6A-07A4-4982-8BC0-63F905116036}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB8D833B-D0DE-493A-A475-EF009E87BF86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28255,25 +28245,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{117D62C5-B693-4014-B24B-9D6D08B6151A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
-    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
-    <ds:schemaRef ds:uri="db15119c-9bb3-4b2d-aba7-a20f2bdcd107"/>
-    <ds:schemaRef ds:uri="ce1eb032-f7c0-42b6-914e-65a5c98ce8c4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B327EE6A-07A4-4982-8BC0-63F905116036}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>